<commit_message>
Entire EVE build validated except alignment tree
</commit_message>
<xml_diff>
--- a/tabular/eve/efv-reference_feature_locations.xlsx
+++ b/tabular/eve/efv-reference_feature_locations.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/RNA+ve/Flaviviridae-GLUE/tabular/eve/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46E108B-B6E2-2E43-BEE2-18E47CF76AC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -175,19 +181,19 @@
     <t>whole_genome</t>
   </si>
   <si>
-    <t>EFV-Pestinsect.3-Ceratina-con</t>
+    <t>Pestinsect</t>
   </si>
   <si>
-    <t>REF_EFV_PI3_Ceratina</t>
+    <t>EFV-PL2.3-CerCal</t>
   </si>
   <si>
-    <t>Pestinsect</t>
+    <t>REF_EFV-PL2.3-CerCal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -248,7 +254,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +309,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2432,7 +2444,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2459,6 +2471,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2117">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -4913,14 +4926,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1441"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G3" sqref="A1:G3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
@@ -4931,7 +4944,7 @@
     <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -4954,15 +4967,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="7" t="s">
@@ -4975,15 +4988,15 @@
         <v>14403</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="7" t="s">
@@ -4996,819 +5009,819 @@
         <v>14403</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C4"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5"/>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6"/>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C7"/>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11"/>
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12"/>
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14"/>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C16"/>
       <c r="D16"/>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="3:4">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="3:4">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C21"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="3:4">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C22"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="3:4">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C23"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="3:4">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="3:4">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C25"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="3:4" ht="16" customHeight="1">
+    <row r="26" spans="3:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="3:4">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="3:4">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C28"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="3:4">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C29"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="3:4">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="3:4">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C31"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="3:4">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C32"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="3:4">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="3:4">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C34"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="3:4">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C35"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="3:4">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="3:4">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C37"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="3:4">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C38"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="3:4">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C39"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="3:4">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C40"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="3:4">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C41"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="3:4">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C42"/>
       <c r="D42"/>
     </row>
-    <row r="43" spans="3:4">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C43"/>
       <c r="D43"/>
     </row>
-    <row r="44" spans="3:4">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C44"/>
       <c r="D44"/>
     </row>
-    <row r="45" spans="3:4">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C45"/>
       <c r="D45"/>
     </row>
-    <row r="46" spans="3:4">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C46"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="3:4">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C47"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="3:4">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C48"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="3:4">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C49"/>
       <c r="D49"/>
     </row>
-    <row r="50" spans="3:4">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C50"/>
       <c r="D50"/>
     </row>
-    <row r="51" spans="3:4">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C51"/>
       <c r="D51"/>
     </row>
-    <row r="52" spans="3:4">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C52"/>
       <c r="D52"/>
     </row>
-    <row r="53" spans="3:4">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C53"/>
       <c r="D53"/>
     </row>
-    <row r="54" spans="3:4">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C54"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="3:4">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C55"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="3:4">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C56"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="3:4">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C57"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="3:4">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C58"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="3:4">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C59"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="3:4">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C60"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="3:4">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C61"/>
       <c r="D61"/>
     </row>
-    <row r="62" spans="3:4">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C62"/>
       <c r="D62"/>
     </row>
-    <row r="63" spans="3:4">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C63"/>
       <c r="D63"/>
     </row>
-    <row r="64" spans="3:4">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C64"/>
       <c r="D64"/>
     </row>
-    <row r="65" spans="3:4">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C65"/>
       <c r="D65"/>
     </row>
-    <row r="66" spans="3:4">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C66"/>
       <c r="D66"/>
     </row>
-    <row r="67" spans="3:4">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C67"/>
       <c r="D67"/>
     </row>
-    <row r="68" spans="3:4">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C68"/>
       <c r="D68"/>
     </row>
-    <row r="69" spans="3:4">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C69"/>
       <c r="D69"/>
     </row>
-    <row r="70" spans="3:4">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C70"/>
       <c r="D70"/>
     </row>
-    <row r="71" spans="3:4">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C71"/>
       <c r="D71"/>
     </row>
-    <row r="72" spans="3:4">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C72"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="3:4">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C73"/>
       <c r="D73"/>
     </row>
-    <row r="74" spans="3:4">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C74"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="3:4">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C75"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="3:4">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C76"/>
       <c r="D76"/>
     </row>
-    <row r="77" spans="3:4">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C77"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="3:4">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C78"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="3:4">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C79"/>
       <c r="D79"/>
     </row>
-    <row r="80" spans="3:4">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C80"/>
       <c r="D80"/>
     </row>
-    <row r="81" spans="3:4">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C81"/>
       <c r="D81"/>
     </row>
-    <row r="82" spans="3:4">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C82"/>
       <c r="D82"/>
     </row>
-    <row r="83" spans="3:4">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C83"/>
       <c r="D83"/>
     </row>
-    <row r="84" spans="3:4">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C84"/>
       <c r="D84"/>
     </row>
-    <row r="85" spans="3:4">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C85"/>
       <c r="D85"/>
     </row>
-    <row r="86" spans="3:4">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C86"/>
       <c r="D86"/>
     </row>
-    <row r="87" spans="3:4">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C87"/>
       <c r="D87"/>
     </row>
-    <row r="88" spans="3:4">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C88"/>
       <c r="D88"/>
     </row>
-    <row r="89" spans="3:4">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C89"/>
       <c r="D89"/>
     </row>
-    <row r="90" spans="3:4">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C90"/>
       <c r="D90"/>
     </row>
-    <row r="91" spans="3:4">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C91"/>
       <c r="D91"/>
     </row>
-    <row r="92" spans="3:4">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C92"/>
       <c r="D92"/>
     </row>
-    <row r="93" spans="3:4">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C93"/>
       <c r="D93"/>
     </row>
-    <row r="94" spans="3:4">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C94"/>
       <c r="D94"/>
     </row>
-    <row r="95" spans="3:4">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C95"/>
       <c r="D95"/>
     </row>
-    <row r="96" spans="3:4">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C96"/>
       <c r="D96"/>
     </row>
-    <row r="97" spans="3:4">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C97"/>
       <c r="D97"/>
     </row>
-    <row r="98" spans="3:4">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C98"/>
       <c r="D98"/>
     </row>
-    <row r="99" spans="3:4">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C99"/>
       <c r="D99"/>
     </row>
-    <row r="100" spans="3:4">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C100"/>
       <c r="D100"/>
     </row>
-    <row r="101" spans="3:4">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C101"/>
       <c r="D101"/>
     </row>
-    <row r="102" spans="3:4">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C102"/>
       <c r="D102"/>
     </row>
-    <row r="103" spans="3:4">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C103"/>
       <c r="D103"/>
     </row>
-    <row r="104" spans="3:4">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C104"/>
       <c r="D104"/>
     </row>
-    <row r="105" spans="3:4">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C105"/>
       <c r="D105"/>
     </row>
-    <row r="106" spans="3:4">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C106"/>
       <c r="D106"/>
     </row>
-    <row r="107" spans="3:4">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C107"/>
       <c r="D107"/>
     </row>
-    <row r="108" spans="3:4">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C108"/>
       <c r="D108"/>
     </row>
-    <row r="109" spans="3:4">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C109"/>
       <c r="D109"/>
     </row>
-    <row r="110" spans="3:4">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C110"/>
       <c r="D110"/>
     </row>
-    <row r="111" spans="3:4">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C111"/>
       <c r="D111"/>
     </row>
-    <row r="112" spans="3:4">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C112"/>
       <c r="D112"/>
     </row>
-    <row r="113" spans="3:4">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C113"/>
       <c r="D113"/>
     </row>
-    <row r="114" spans="3:4">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C114"/>
       <c r="D114"/>
     </row>
-    <row r="115" spans="3:4">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C115"/>
       <c r="D115"/>
     </row>
-    <row r="116" spans="3:4">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C116"/>
       <c r="D116"/>
     </row>
-    <row r="117" spans="3:4">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C117"/>
       <c r="D117"/>
     </row>
-    <row r="118" spans="3:4">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C118"/>
       <c r="D118"/>
     </row>
-    <row r="119" spans="3:4">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C119"/>
       <c r="D119"/>
     </row>
-    <row r="120" spans="3:4">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C120"/>
       <c r="D120"/>
     </row>
-    <row r="121" spans="3:4">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C121"/>
       <c r="D121"/>
     </row>
-    <row r="122" spans="3:4">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C122"/>
       <c r="D122"/>
     </row>
-    <row r="123" spans="3:4">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C123"/>
       <c r="D123"/>
     </row>
-    <row r="163" spans="2:4">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B163" s="1"/>
       <c r="C163" s="5"/>
       <c r="D163" s="5"/>
     </row>
-    <row r="164" spans="2:4">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B164" s="1"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
     </row>
-    <row r="165" spans="2:4">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B165" s="1"/>
       <c r="C165" s="5"/>
       <c r="D165" s="5"/>
     </row>
-    <row r="166" spans="2:4">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B166" s="1"/>
       <c r="C166" s="5"/>
       <c r="D166" s="5"/>
     </row>
-    <row r="167" spans="2:4">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B167" s="1"/>
       <c r="C167" s="5"/>
       <c r="D167" s="5"/>
     </row>
-    <row r="168" spans="2:4">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B168" s="1"/>
       <c r="C168" s="5"/>
       <c r="D168" s="5"/>
     </row>
-    <row r="169" spans="2:4">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B169" s="1"/>
       <c r="C169" s="5"/>
       <c r="D169" s="5"/>
     </row>
-    <row r="170" spans="2:4">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B170" s="1"/>
       <c r="C170" s="5"/>
       <c r="D170" s="5"/>
     </row>
-    <row r="171" spans="2:4">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B171" s="1"/>
       <c r="C171" s="5"/>
       <c r="D171" s="5"/>
     </row>
-    <row r="172" spans="2:4">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B172" s="1"/>
       <c r="C172" s="5"/>
       <c r="D172" s="5"/>
     </row>
-    <row r="173" spans="2:4">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B173" s="1"/>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
     </row>
-    <row r="174" spans="2:4">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B174" s="1"/>
       <c r="C174" s="5"/>
       <c r="D174" s="5"/>
     </row>
-    <row r="175" spans="2:4">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B175" s="1"/>
       <c r="C175" s="5"/>
       <c r="D175" s="5"/>
     </row>
-    <row r="176" spans="2:4">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B176" s="1"/>
       <c r="C176" s="5"/>
       <c r="D176" s="5"/>
     </row>
-    <row r="177" spans="2:4">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B177" s="1"/>
       <c r="C177" s="5"/>
       <c r="D177" s="5"/>
     </row>
-    <row r="178" spans="2:4">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B178" s="1"/>
       <c r="C178" s="5"/>
       <c r="D178" s="5"/>
     </row>
-    <row r="179" spans="2:4">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B179" s="1"/>
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
     </row>
-    <row r="180" spans="2:4">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B180" s="1"/>
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
     </row>
-    <row r="181" spans="2:4">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B181" s="1"/>
       <c r="C181" s="5"/>
       <c r="D181" s="5"/>
     </row>
-    <row r="182" spans="2:4">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B182" s="1"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
     </row>
-    <row r="183" spans="2:4">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B183" s="1"/>
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
     </row>
-    <row r="184" spans="2:4">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B184" s="1"/>
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
     </row>
-    <row r="185" spans="2:4">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B185" s="1"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
     </row>
-    <row r="186" spans="2:4">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B186" s="1"/>
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
     </row>
-    <row r="187" spans="2:4">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B187" s="1"/>
     </row>
-    <row r="188" spans="2:4">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B188" s="1"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
     </row>
-    <row r="189" spans="2:4">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B189" s="1"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
     </row>
-    <row r="190" spans="2:4">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B190" s="1"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
     </row>
-    <row r="191" spans="2:4">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B191" s="1"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
     </row>
-    <row r="192" spans="2:4">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B192" s="1"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
     </row>
-    <row r="193" spans="2:4">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B193" s="1"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
     </row>
-    <row r="194" spans="2:4">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B194" s="1"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
     </row>
-    <row r="877" spans="5:5">
+    <row r="877" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E877" s="1"/>
     </row>
-    <row r="1013" spans="2:2">
+    <row r="1013" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1013" s="1"/>
     </row>
-    <row r="1014" spans="2:2">
+    <row r="1014" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1014" s="1"/>
     </row>
-    <row r="1139" spans="2:2">
+    <row r="1139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1139" s="1"/>
     </row>
-    <row r="1140" spans="2:2">
+    <row r="1140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1140" s="1"/>
     </row>
-    <row r="1141" spans="2:2">
+    <row r="1141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1141" s="1"/>
     </row>
-    <row r="1142" spans="2:2">
+    <row r="1142" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1142" s="1"/>
     </row>
-    <row r="1143" spans="2:2">
+    <row r="1143" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1143" s="1"/>
     </row>
-    <row r="1144" spans="2:2">
+    <row r="1144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1144" s="1"/>
     </row>
-    <row r="1189" spans="2:6">
+    <row r="1189" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1189" s="1"/>
       <c r="F1189" s="1"/>
     </row>
-    <row r="1190" spans="2:6">
+    <row r="1190" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1190" s="1"/>
       <c r="F1190" s="1"/>
     </row>
-    <row r="1191" spans="2:6">
+    <row r="1191" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1191" s="1"/>
       <c r="F1191" s="1"/>
     </row>
-    <row r="1193" spans="2:6">
+    <row r="1193" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1193" s="1"/>
     </row>
-    <row r="1194" spans="2:6">
+    <row r="1194" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1194" s="1"/>
     </row>
-    <row r="1195" spans="2:6">
+    <row r="1195" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1195" s="1"/>
     </row>
-    <row r="1196" spans="2:6">
+    <row r="1196" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1196" s="1"/>
     </row>
-    <row r="1197" spans="2:6">
+    <row r="1197" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1197" s="1"/>
     </row>
-    <row r="1216" spans="2:2">
+    <row r="1216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1216" s="1"/>
     </row>
-    <row r="1217" spans="2:2">
+    <row r="1217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1217" s="1"/>
     </row>
-    <row r="1218" spans="2:2">
+    <row r="1218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1218" s="1"/>
     </row>
-    <row r="1219" spans="2:2">
+    <row r="1219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1219" s="1"/>
     </row>
-    <row r="1220" spans="2:2">
+    <row r="1220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1220" s="1"/>
     </row>
-    <row r="1221" spans="2:2">
+    <row r="1221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1221" s="1"/>
     </row>
-    <row r="1222" spans="2:2">
+    <row r="1222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1222" s="1"/>
     </row>
-    <row r="1224" spans="2:2">
+    <row r="1224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1224" s="1"/>
     </row>
-    <row r="1225" spans="2:2">
+    <row r="1225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1225" s="1"/>
     </row>
-    <row r="1226" spans="2:2">
+    <row r="1226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1226" s="1"/>
     </row>
-    <row r="1227" spans="2:2">
+    <row r="1227" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1227" s="1"/>
     </row>
-    <row r="1228" spans="2:2">
+    <row r="1228" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1228" s="1"/>
     </row>
-    <row r="1229" spans="2:2">
+    <row r="1229" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1229" s="1"/>
     </row>
-    <row r="1281" spans="2:2">
+    <row r="1281" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1281" s="1"/>
     </row>
-    <row r="1282" spans="2:2">
+    <row r="1282" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1282" s="1"/>
     </row>
-    <row r="1283" spans="2:2">
+    <row r="1283" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1283" s="1"/>
     </row>
-    <row r="1284" spans="2:2">
+    <row r="1284" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1284" s="1"/>
     </row>
-    <row r="1286" spans="2:2">
+    <row r="1286" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1286" s="1"/>
     </row>
-    <row r="1287" spans="2:2">
+    <row r="1287" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1287" s="1"/>
     </row>
-    <row r="1288" spans="2:2">
+    <row r="1288" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1288" s="1"/>
     </row>
-    <row r="1289" spans="2:2">
+    <row r="1289" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1289" s="1"/>
     </row>
-    <row r="1324" spans="2:2">
+    <row r="1324" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1324" s="1"/>
     </row>
-    <row r="1325" spans="2:2">
+    <row r="1325" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1325" s="1"/>
     </row>
-    <row r="1326" spans="2:2">
+    <row r="1326" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1326" s="1"/>
     </row>
-    <row r="1327" spans="2:2">
+    <row r="1327" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1327" s="1"/>
     </row>
-    <row r="1328" spans="2:2">
+    <row r="1328" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1328" s="1"/>
     </row>
-    <row r="1329" spans="2:2">
+    <row r="1329" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1329" s="1"/>
     </row>
-    <row r="1371" spans="3:6">
+    <row r="1371" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E1371" s="1"/>
       <c r="F1371" s="1"/>
     </row>
-    <row r="1372" spans="3:6">
+    <row r="1372" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1372" s="6"/>
       <c r="D1372" s="6"/>
       <c r="E1372" s="1"/>
       <c r="F1372" s="1"/>
     </row>
-    <row r="1373" spans="3:6">
+    <row r="1373" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1373" s="6"/>
       <c r="D1373" s="6"/>
       <c r="E1373" s="1"/>
       <c r="F1373" s="1"/>
     </row>
-    <row r="1374" spans="3:6">
+    <row r="1374" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1374" s="6"/>
       <c r="D1374" s="6"/>
       <c r="E1374" s="1"/>
       <c r="F1374" s="1"/>
     </row>
-    <row r="1375" spans="3:6">
+    <row r="1375" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E1375" s="1"/>
       <c r="F1375" s="1"/>
     </row>
-    <row r="1438" spans="2:2">
+    <row r="1438" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1438" s="1"/>
     </row>
-    <row r="1439" spans="2:2">
+    <row r="1439" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1439" s="1"/>
     </row>
-    <row r="1440" spans="2:2">
+    <row r="1440" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1440" s="1"/>
     </row>
-    <row r="1441" spans="2:2">
+    <row r="1441" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1441" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:H1495">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H1495">
     <sortCondition ref="C2:C1495"/>
     <sortCondition ref="D2:D1495"/>
   </sortState>
@@ -5823,16 +5836,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G43" sqref="A28:G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -5855,7 +5868,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -5878,7 +5891,7 @@
         <v>10389</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -5901,7 +5914,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -5924,7 +5937,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -5947,7 +5960,7 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -5970,7 +5983,7 @@
         <v>3513</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -5993,7 +6006,7 @@
         <v>4206</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -6016,7 +6029,7 @@
         <v>4599</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -6039,7 +6052,7 @@
         <v>6456</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -6062,7 +6075,7 @@
         <v>6903</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -6085,7 +6098,7 @@
         <v>7671</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -6108,7 +6121,7 @@
         <v>10386</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -6131,7 +6144,7 @@
         <v>10962</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -6154,7 +6167,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -6177,7 +6190,7 @@
         <v>10366</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -6200,7 +6213,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -6223,7 +6236,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -6246,7 +6259,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -6269,7 +6282,7 @@
         <v>3532</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -6292,7 +6305,7 @@
         <v>4210</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14" customHeight="1">
+    <row r="21" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -6315,7 +6328,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -6338,7 +6351,7 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -6361,7 +6374,7 @@
         <v>6832</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -6384,7 +6397,7 @@
         <v>6901</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -6407,7 +6420,7 @@
         <v>7654</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -6430,7 +6443,7 @@
         <v>10363</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -6453,7 +6466,7 @@
         <v>10794</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -6476,7 +6489,7 @@
         <v>10116</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -6499,7 +6512,7 @@
         <v>10242</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -6519,7 +6532,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -6539,7 +6552,7 @@
         <v>12352</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -6559,7 +6572,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -6579,7 +6592,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -6599,7 +6612,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -6619,7 +6632,7 @@
         <v>2461</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -6639,7 +6652,7 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -6659,7 +6672,7 @@
         <v>3793</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>27</v>
       </c>
@@ -6679,7 +6692,7 @@
         <v>7471</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>27</v>
       </c>
@@ -6699,7 +6712,7 @@
         <v>7663</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>27</v>
       </c>
@@ -6719,7 +6732,7 @@
         <v>8704</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>27</v>
       </c>
@@ -6739,7 +6752,7 @@
         <v>10192</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -6759,7 +6772,7 @@
         <v>12349</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -6779,7 +6792,7 @@
         <v>12573</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -6802,7 +6815,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -6825,7 +6838,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -6848,7 +6861,7 @@
         <v>2849</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>36</v>
       </c>

</xml_diff>